<commit_message>
Cambios en Login, en Clase empresas, logica y test, cambio en menu
</commit_message>
<xml_diff>
--- a/Datos/testdata.xlsx
+++ b/Datos/testdata.xlsx
@@ -8,7 +8,7 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="empresa" r:id="rId2" sheetId="1" state="visible"/>
+    <sheet name="Empresas" r:id="rId2" sheetId="1" state="visible"/>
     <sheet name="usuarios" r:id="rId3" sheetId="2" state="visible"/>
     <sheet name="reportes" r:id="rId4" sheetId="3" state="visible"/>
   </sheets>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="73">
   <si>
     <t xml:space="preserve">Test Case Name</t>
   </si>
@@ -381,7 +381,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
+      <selection activeCell="C4" activeCellId="0" pane="topLeft" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>

</xml_diff>